<commit_message>
updated creation of histogram with AAIMON for each protein
</commit_message>
<xml_diff>
--- a/korbinian/examples/settings/korbinian_run_settings_schweris.xlsx
+++ b/korbinian/examples/settings/korbinian_run_settings_schweris.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="3090" yWindow="2955" windowWidth="14265" windowHeight="7860"/>
+    <workbookView xWindow="3090" yWindow="3135" windowWidth="14265" windowHeight="7680"/>
   </bookViews>
   <sheets>
     <sheet name="run_settings" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="219">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="221">
   <si>
     <t>uniprot_list</t>
   </si>
@@ -225,9 +225,6 @@
     <t>""</t>
   </si>
   <si>
-    <t>main_folder</t>
-  </si>
-  <si>
     <t>eaSimap_path</t>
   </si>
   <si>
@@ -378,9 +375,6 @@
     <t>D:\Databases</t>
   </si>
   <si>
-    <t>D:\Databases\main</t>
-  </si>
-  <si>
     <t>list_of_uniprot_accessions</t>
   </si>
   <si>
@@ -426,12 +420,6 @@
     <t>cr_maximum_identity_of_full_protein</t>
   </si>
   <si>
-    <t>cr_mimimum_length_match_sequence</t>
-  </si>
-  <si>
-    <t>cr_mimimum_length_non_TMD_sequence</t>
-  </si>
-  <si>
     <t>cr_randomised_tmd</t>
   </si>
   <si>
@@ -486,9 +474,6 @@
     <t>your_name</t>
   </si>
   <si>
-    <t>Jakob Maria Mierscheid</t>
-  </si>
-  <si>
     <t>ASCII text! Identifier to determine who downloaded SIMAP homologues</t>
   </si>
   <si>
@@ -673,6 +658,27 @@
   </si>
   <si>
     <t>cr_max_identity_of_full_protein</t>
+  </si>
+  <si>
+    <t>Mark Teese</t>
+  </si>
+  <si>
+    <t>run_gather_AAIMON_ratios</t>
+  </si>
+  <si>
+    <t>overwrite_simap_parsed_to_csv</t>
+  </si>
+  <si>
+    <t>analyse_signal_peptides</t>
+  </si>
+  <si>
+    <t>cr_minimum_length_match_sequence</t>
+  </si>
+  <si>
+    <t>cr_minimum_length_non_TMD_sequence</t>
+  </si>
+  <si>
+    <t>not in use</t>
   </si>
 </sst>
 </file>
@@ -868,7 +874,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="83">
+  <cellXfs count="82">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1031,9 +1037,6 @@
     <xf numFmtId="0" fontId="0" fillId="23" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="23" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="24" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="24" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1052,7 +1055,119 @@
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="29">
+  <dxfs count="45">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1562,15 +1677,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C43"/>
+  <dimension ref="A1:C44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="66" style="1" customWidth="1"/>
+    <col min="1" max="1" width="59.42578125" style="1" customWidth="1"/>
     <col min="2" max="2" width="7.85546875" style="4" customWidth="1"/>
     <col min="3" max="3" width="85.5703125" style="1" customWidth="1"/>
     <col min="4" max="16384" width="9.140625" style="1"/>
@@ -1578,7 +1693,7 @@
   <sheetData>
     <row r="1" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B1" s="13" t="s">
         <v>59</v>
@@ -1589,7 +1704,7 @@
     </row>
     <row r="2" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="16" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B2" s="36"/>
       <c r="C2" s="53"/>
@@ -1599,7 +1714,7 @@
         <v>0</v>
       </c>
       <c r="B3" s="37">
-        <v>92</v>
+        <v>12</v>
       </c>
       <c r="C3" s="54" t="s">
         <v>9</v>
@@ -1632,42 +1747,42 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="26" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="B7" s="48"/>
       <c r="C7" s="27"/>
     </row>
     <row r="8" spans="1:3" s="63" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="28" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="B8" s="70" t="s">
         <v>8</v>
       </c>
       <c r="C8" s="29" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
     </row>
     <row r="9" spans="1:3" s="63" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="28" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="B9" s="70" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="C9" s="29" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
     </row>
     <row r="10" spans="1:3" s="63" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="28" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="B10" s="70" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="C10" s="29" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -1676,14 +1791,14 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="18" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="B12" s="39"/>
       <c r="C12" s="55"/>
     </row>
     <row r="13" spans="1:3" s="63" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="19" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="B13" s="70" t="s">
         <v>8</v>
@@ -1692,7 +1807,7 @@
     </row>
     <row r="14" spans="1:3" s="69" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="B14" s="70" t="s">
         <v>8</v>
@@ -1701,7 +1816,7 @@
     </row>
     <row r="15" spans="1:3" s="67" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="31" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="B15" s="70" t="s">
         <v>8</v>
@@ -1710,7 +1825,7 @@
     </row>
     <row r="16" spans="1:3" s="63" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="19" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B16" s="70" t="s">
         <v>8</v>
@@ -1721,7 +1836,7 @@
     </row>
     <row r="17" spans="1:3" s="69" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="9" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B17" s="70" t="s">
         <v>8</v>
@@ -1732,7 +1847,7 @@
     </row>
     <row r="18" spans="1:3" s="67" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="31" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B18" s="70" t="s">
         <v>8</v>
@@ -1743,10 +1858,10 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="19" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B19" s="70" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C19" s="56" t="s">
         <v>15</v>
@@ -1754,10 +1869,10 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="31" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="B20" s="70" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C20" s="32" t="s">
         <v>16</v>
@@ -1769,17 +1884,17 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="22" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B22" s="41"/>
       <c r="C22" s="57"/>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="64" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B23" s="70" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C23" s="65" t="s">
         <v>17</v>
@@ -1787,10 +1902,10 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="66" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B24" s="70" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C24" s="66" t="s">
         <v>18</v>
@@ -1802,28 +1917,28 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="24" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B26" s="43"/>
       <c r="C26" s="59"/>
     </row>
     <row r="27" spans="1:3" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="6" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="B27" s="70" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C27" s="25" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
     </row>
     <row r="28" spans="1:3" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="6" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="B28" s="70" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C28" s="25" t="s">
         <v>62</v>
@@ -1831,10 +1946,10 @@
     </row>
     <row r="29" spans="1:3" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="6" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B29" s="70" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C29" s="25" t="s">
         <v>62</v>
@@ -1842,85 +1957,85 @@
     </row>
     <row r="30" spans="1:3" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="6" t="s">
+        <v>215</v>
+      </c>
+      <c r="B30" s="70" t="s">
+        <v>7</v>
+      </c>
+      <c r="C30" s="25" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="B31" s="70" t="s">
+        <v>8</v>
+      </c>
+      <c r="C31" s="25" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="62"/>
+      <c r="B32" s="4"/>
+      <c r="C32" s="62"/>
+    </row>
+    <row r="33" spans="1:3" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="20" t="s">
+        <v>94</v>
+      </c>
+      <c r="B33" s="45"/>
+      <c r="C33" s="60"/>
+    </row>
+    <row r="34" spans="1:3" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="21" t="s">
         <v>104</v>
       </c>
-      <c r="B30" s="70" t="s">
-        <v>8</v>
-      </c>
-      <c r="C30" s="25" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="62"/>
-      <c r="B31" s="4"/>
-      <c r="C31" s="62"/>
-    </row>
-    <row r="32" spans="1:3" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="20" t="s">
+      <c r="B34" s="70" t="s">
+        <v>8</v>
+      </c>
+      <c r="C34" s="61" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="21" t="s">
+        <v>105</v>
+      </c>
+      <c r="B35" s="70" t="s">
+        <v>8</v>
+      </c>
+      <c r="C35" s="61" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" s="21" t="s">
+        <v>106</v>
+      </c>
+      <c r="B36" s="70" t="s">
+        <v>8</v>
+      </c>
+      <c r="C36" s="61" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" s="62"/>
+      <c r="C37" s="62"/>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" s="26" t="s">
         <v>95</v>
       </c>
-      <c r="B32" s="45"/>
-      <c r="C32" s="60"/>
-    </row>
-    <row r="33" spans="1:3" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="21" t="s">
-        <v>105</v>
-      </c>
-      <c r="B33" s="70" t="s">
-        <v>8</v>
-      </c>
-      <c r="C33" s="61" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="21" t="s">
-        <v>106</v>
-      </c>
-      <c r="B34" s="70" t="s">
-        <v>8</v>
-      </c>
-      <c r="C34" s="61" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" s="21" t="s">
-        <v>107</v>
-      </c>
-      <c r="B35" s="70" t="s">
-        <v>8</v>
-      </c>
-      <c r="C35" s="61" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" s="62"/>
-      <c r="C36" s="62"/>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" s="26" t="s">
-        <v>96</v>
-      </c>
-      <c r="B37" s="48"/>
-      <c r="C37" s="27"/>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" s="28" t="s">
-        <v>108</v>
-      </c>
-      <c r="B38" s="70" t="s">
-        <v>8</v>
-      </c>
-      <c r="C38" s="29" t="s">
-        <v>21</v>
-      </c>
+      <c r="B38" s="48"/>
+      <c r="C38" s="27"/>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="28" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B39" s="70" t="s">
         <v>8</v>
@@ -1931,7 +2046,7 @@
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="28" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B40" s="70" t="s">
         <v>8</v>
@@ -1942,7 +2057,7 @@
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="28" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="B41" s="70" t="s">
         <v>8</v>
@@ -1953,7 +2068,7 @@
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="28" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="B42" s="70" t="s">
         <v>8</v>
@@ -1964,7 +2079,7 @@
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="28" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B43" s="70" t="s">
         <v>8</v>
@@ -1973,100 +2088,116 @@
         <v>21</v>
       </c>
     </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" s="28" t="s">
+        <v>111</v>
+      </c>
+      <c r="B44" s="70" t="s">
+        <v>8</v>
+      </c>
+      <c r="C44" s="29" t="s">
+        <v>21</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="B1 B6 B44:B1048576">
-    <cfRule type="containsText" dxfId="28" priority="234" operator="containsText" text="TRUE">
+  <conditionalFormatting sqref="B1 B6 B45:B1048576">
+    <cfRule type="containsText" dxfId="44" priority="283" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",B1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B21">
-    <cfRule type="containsText" dxfId="27" priority="232" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="43" priority="281" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",B21)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B25">
-    <cfRule type="containsText" dxfId="26" priority="231" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="42" priority="280" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",B25)))</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="B32">
+    <cfRule type="containsText" dxfId="41" priority="279" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",B32)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B37">
+    <cfRule type="containsText" dxfId="40" priority="278" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",B37)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B39:B44 B34 B36 B16:B17">
+    <cfRule type="containsText" dxfId="39" priority="277" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",B16)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B35">
+    <cfRule type="containsText" dxfId="38" priority="267" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",B35)))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="B31">
-    <cfRule type="containsText" dxfId="25" priority="230" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="37" priority="210" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",B31)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B36">
-    <cfRule type="containsText" dxfId="24" priority="229" operator="containsText" text="TRUE">
-      <formula>NOT(ISERROR(SEARCH("TRUE",B36)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B38:B43 B33 B35 B16:B17">
-    <cfRule type="containsText" dxfId="23" priority="228" operator="containsText" text="TRUE">
-      <formula>NOT(ISERROR(SEARCH("TRUE",B16)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B34">
-    <cfRule type="containsText" dxfId="22" priority="218" operator="containsText" text="TRUE">
-      <formula>NOT(ISERROR(SEARCH("TRUE",B34)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B30">
-    <cfRule type="containsText" dxfId="21" priority="161" operator="containsText" text="TRUE">
-      <formula>NOT(ISERROR(SEARCH("TRUE",B30)))</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="B18">
-    <cfRule type="containsText" dxfId="20" priority="152" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="36" priority="201" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",B18)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B13:B15">
-    <cfRule type="containsText" dxfId="19" priority="68" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="35" priority="117" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",B13)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B8:B10">
-    <cfRule type="containsText" dxfId="18" priority="37" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="34" priority="86" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",B8)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B11">
-    <cfRule type="containsText" dxfId="17" priority="36" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="33" priority="85" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",B11)))</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="B23">
+    <cfRule type="containsText" dxfId="32" priority="49" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",B23)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B30">
+    <cfRule type="containsText" dxfId="31" priority="44" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",B30)))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="B29">
-    <cfRule type="containsText" dxfId="16" priority="13" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="26" priority="14" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",B29)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B28">
-    <cfRule type="containsText" dxfId="15" priority="8" operator="containsText" text="TRUE">
-      <formula>NOT(ISERROR(SEARCH("TRUE",B28)))</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="B19">
-    <cfRule type="containsText" dxfId="9" priority="5" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="13" priority="7" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",B19)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B20">
-    <cfRule type="containsText" dxfId="7" priority="4" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="11" priority="6" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",B20)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B23">
-    <cfRule type="containsText" dxfId="5" priority="3" operator="containsText" text="TRUE">
-      <formula>NOT(ISERROR(SEARCH("TRUE",B23)))</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="B24">
-    <cfRule type="containsText" dxfId="3" priority="2" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="9" priority="5" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",B24)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B27">
+    <cfRule type="containsText" dxfId="7" priority="4" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",B27)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B28">
     <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="TRUE">
-      <formula>NOT(ISERROR(SEARCH("TRUE",B27)))</formula>
+      <formula>NOT(ISERROR(SEARCH("TRUE",B28)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2079,7 +2210,7 @@
   <dimension ref="A1:C23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2091,7 +2222,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B1" s="13" t="s">
         <v>59</v>
@@ -2102,13 +2233,13 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="B2" t="s">
-        <v>156</v>
+        <v>214</v>
       </c>
       <c r="C2" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -2116,7 +2247,7 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -2124,169 +2255,177 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="B5" t="s">
-        <v>120</v>
+        <v>168</v>
+      </c>
+      <c r="C5" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B6" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="C6" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>70</v>
+        <v>165</v>
       </c>
       <c r="B7" t="s">
-        <v>174</v>
-      </c>
-      <c r="C7" t="s">
-        <v>71</v>
+        <v>170</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
       <c r="B8" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="B9" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
       <c r="B10" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+        <v>173</v>
+      </c>
+      <c r="C10" t="s">
         <v>163</v>
       </c>
-      <c r="B11" t="s">
-        <v>178</v>
-      </c>
-      <c r="C11" t="s">
-        <v>168</v>
-      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="18" t="s">
+        <v>191</v>
+      </c>
+      <c r="B12" s="39"/>
+      <c r="C12" s="55"/>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="18" t="s">
-        <v>196</v>
-      </c>
-      <c r="B13" s="39"/>
-      <c r="C13" s="55"/>
+      <c r="A13" t="s">
+        <v>161</v>
+      </c>
+      <c r="B13" t="s">
+        <v>174</v>
+      </c>
+      <c r="C13" t="s">
+        <v>162</v>
+      </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>166</v>
+        <v>119</v>
       </c>
       <c r="B14" t="s">
-        <v>179</v>
-      </c>
-      <c r="C14" t="s">
-        <v>167</v>
+        <v>120</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>121</v>
-      </c>
-      <c r="B15" t="s">
-        <v>122</v>
+        <v>175</v>
+      </c>
+      <c r="B15" s="70" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>176</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>180</v>
+        <v>217</v>
       </c>
       <c r="B16" s="70" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="18" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="B18" s="39"/>
       <c r="C18" s="55"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="B19" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="B20" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
+        <v>181</v>
+      </c>
+      <c r="B21" t="s">
         <v>186</v>
-      </c>
-      <c r="B21" t="s">
-        <v>191</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
+        <v>182</v>
+      </c>
+      <c r="B22" t="s">
         <v>187</v>
-      </c>
-      <c r="B22" t="s">
-        <v>192</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
+        <v>188</v>
+      </c>
+      <c r="B23" t="s">
         <v>193</v>
       </c>
-      <c r="B23" t="s">
-        <v>198</v>
-      </c>
       <c r="C23" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B1">
-    <cfRule type="containsText" dxfId="12" priority="2" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="24" priority="3" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",B1)))</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="B15">
+    <cfRule type="containsText" dxfId="23" priority="2" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",B15)))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="B16">
-    <cfRule type="containsText" dxfId="11" priority="1" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="21" priority="1" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",B16)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2297,10 +2436,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C98"/>
+  <dimension ref="A1:C99"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="B29" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2312,7 +2451,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B1" s="35" t="s">
         <v>59</v>
@@ -2323,7 +2462,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="16" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B2" s="36"/>
       <c r="C2" s="53"/>
@@ -2374,163 +2513,163 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="18" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B8" s="39"/>
       <c r="C8" s="55"/>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="19" t="s">
-        <v>27</v>
-      </c>
-      <c r="B9" s="40" t="s">
-        <v>7</v>
+        <v>28</v>
+      </c>
+      <c r="B9" s="40" t="b">
+        <v>0</v>
       </c>
       <c r="C9" s="56"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="B10" s="40" t="b">
-        <v>0</v>
+        <v>29</v>
+      </c>
+      <c r="B10" s="40" t="s">
+        <v>8</v>
       </c>
       <c r="C10" s="56"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="19" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B11" s="40" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C11" s="56"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="19" t="s">
-        <v>30</v>
-      </c>
-      <c r="B12" s="40" t="s">
-        <v>7</v>
-      </c>
-      <c r="C12" s="56"/>
+        <v>49</v>
+      </c>
+      <c r="B12" s="40">
+        <v>3000</v>
+      </c>
+      <c r="C12" s="56" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="19" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B13" s="40">
-        <v>3000</v>
-      </c>
-      <c r="C13" s="56" t="s">
-        <v>61</v>
-      </c>
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="C13" s="56"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="19" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B14" s="40">
-        <v>1.0000000000000001E-5</v>
+        <v>5000</v>
       </c>
       <c r="C14" s="56"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="19" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B15" s="40">
-        <v>5000</v>
+        <v>3000</v>
       </c>
       <c r="C15" s="56"/>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="19" t="s">
-        <v>52</v>
-      </c>
-      <c r="B16" s="40">
-        <v>3000</v>
+        <v>53</v>
+      </c>
+      <c r="B16" s="40" t="s">
+        <v>8</v>
       </c>
       <c r="C16" s="56"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="19" t="s">
-        <v>53</v>
+        <v>194</v>
       </c>
       <c r="B17" s="40" t="s">
         <v>8</v>
       </c>
-      <c r="C17" s="56"/>
+      <c r="C17" s="56" t="s">
+        <v>195</v>
+      </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="19" t="s">
-        <v>199</v>
+        <v>54</v>
       </c>
       <c r="B18" s="40" t="s">
-        <v>8</v>
-      </c>
-      <c r="C18" s="56" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="19" t="s">
-        <v>54</v>
-      </c>
-      <c r="B19" s="40" t="s">
         <v>68</v>
       </c>
-      <c r="C19" s="56"/>
-    </row>
-    <row r="20" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="38"/>
-      <c r="C20" s="8"/>
+      <c r="C18" s="56"/>
+    </row>
+    <row r="19" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="38"/>
+      <c r="C19" s="8"/>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="76" t="s">
+        <v>211</v>
+      </c>
+      <c r="B20" s="77"/>
+      <c r="C20" s="78"/>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="77" t="s">
+      <c r="A21" s="79" t="s">
         <v>216</v>
       </c>
-      <c r="B21" s="78"/>
-      <c r="C21" s="79"/>
+      <c r="B21" s="80" t="s">
+        <v>8</v>
+      </c>
+      <c r="C21" s="81"/>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="80" t="s">
-        <v>172</v>
-      </c>
-      <c r="B22" s="81" t="b">
-        <v>0</v>
-      </c>
-      <c r="C22" s="82"/>
+      <c r="A22" s="79" t="s">
+        <v>167</v>
+      </c>
+      <c r="B22" s="80" t="s">
+        <v>8</v>
+      </c>
+      <c r="C22" s="81"/>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="80" t="s">
-        <v>211</v>
-      </c>
-      <c r="B23" s="81" t="s">
+      <c r="A23" s="79" t="s">
+        <v>206</v>
+      </c>
+      <c r="B23" s="80" t="s">
         <v>32</v>
       </c>
-      <c r="C23" s="82"/>
+      <c r="C23" s="81"/>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="80" t="s">
-        <v>212</v>
-      </c>
-      <c r="B24" s="81">
+      <c r="A24" s="79" t="s">
+        <v>207</v>
+      </c>
+      <c r="B24" s="80">
         <v>10</v>
       </c>
-      <c r="C24" s="82" t="s">
-        <v>214</v>
+      <c r="C24" s="81" t="s">
+        <v>209</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="80" t="s">
-        <v>213</v>
-      </c>
-      <c r="B25" s="81">
+      <c r="A25" s="79" t="s">
+        <v>208</v>
+      </c>
+      <c r="B25" s="80">
         <v>10</v>
       </c>
-      <c r="C25" s="82" t="s">
-        <v>215</v>
+      <c r="C25" s="81" t="s">
+        <v>210</v>
       </c>
     </row>
     <row r="26" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.25">
@@ -2539,47 +2678,47 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="22" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="B27" s="41"/>
       <c r="C27" s="57"/>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="23" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="B28" s="42" t="s">
         <v>7</v>
       </c>
       <c r="C28" s="58" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="23" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="B29" s="42" t="s">
         <v>7</v>
       </c>
       <c r="C29" s="58" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="23" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="B30" s="42" t="s">
         <v>7</v>
       </c>
       <c r="C30" s="58" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="23" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="B31" s="42" t="s">
         <v>7</v>
@@ -2588,69 +2727,69 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="23" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="B32" s="42">
-        <v>12</v>
+        <v>60</v>
       </c>
       <c r="C32" s="58" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="23" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="B33" s="42">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="C33" s="58"/>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="23" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="B34" s="42">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="C34" s="58"/>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="23" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B35" s="42" t="s">
         <v>34</v>
       </c>
       <c r="C35" s="58" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="23" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="B36" s="42">
         <v>0.4</v>
       </c>
       <c r="C36" s="58" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="23" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="B37" s="42">
         <v>1</v>
       </c>
       <c r="C37" s="58" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="23" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="B38" s="42" t="s">
         <v>7</v>
@@ -2659,7 +2798,7 @@
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="23" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B39" s="42" t="s">
         <v>8</v>
@@ -2668,13 +2807,13 @@
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="23" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B40" s="42" t="s">
         <v>33</v>
       </c>
       <c r="C40" s="58" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
     </row>
     <row r="41" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.25">
@@ -2683,412 +2822,442 @@
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="71" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="B42" s="72"/>
       <c r="C42" s="73"/>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="74" t="s">
-        <v>129</v>
+        <v>27</v>
       </c>
       <c r="B43" s="75" t="s">
-        <v>33</v>
-      </c>
-      <c r="C43" s="76"/>
+        <v>7</v>
+      </c>
+      <c r="C43" s="75" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="74" t="s">
-        <v>142</v>
-      </c>
-      <c r="B44" s="75">
-        <v>2</v>
-      </c>
-      <c r="C44" s="76"/>
+        <v>127</v>
+      </c>
+      <c r="B44" s="75" t="s">
+        <v>33</v>
+      </c>
+      <c r="C44" s="75" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" s="74" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="B45" s="75">
+        <v>10</v>
+      </c>
+      <c r="C45" s="75">
         <v>2</v>
       </c>
-      <c r="C45" s="76"/>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="74" t="s">
-        <v>217</v>
+        <v>139</v>
       </c>
       <c r="B46" s="75">
-        <v>0.4</v>
-      </c>
-      <c r="C46" s="76"/>
+        <v>10</v>
+      </c>
+      <c r="C46" s="75">
+        <v>2</v>
+      </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" s="74" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="B47" s="75">
-        <v>1</v>
-      </c>
-      <c r="C47" s="76"/>
+        <v>0.4</v>
+      </c>
+      <c r="C47" s="75">
+        <v>0.4</v>
+      </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" s="74" t="s">
-        <v>130</v>
+        <v>213</v>
       </c>
       <c r="B48" s="75">
-        <v>0.3</v>
-      </c>
-      <c r="C48" s="76"/>
+        <v>1</v>
+      </c>
+      <c r="C48" s="75">
+        <v>1</v>
+      </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" s="74" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="B49" s="75">
+        <v>0.2</v>
+      </c>
+      <c r="C49" s="75">
         <v>0.3</v>
       </c>
-      <c r="C49" s="76"/>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" s="74" t="s">
-        <v>132</v>
-      </c>
-      <c r="B50" s="75" t="s">
-        <v>8</v>
-      </c>
-      <c r="C50" s="76"/>
+        <v>129</v>
+      </c>
+      <c r="B50" s="75">
+        <v>0.2</v>
+      </c>
+      <c r="C50" s="75">
+        <v>0.3</v>
+      </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" s="74" t="s">
-        <v>133</v>
-      </c>
-      <c r="B51" s="75">
-        <v>20</v>
-      </c>
-      <c r="C51" s="76"/>
+        <v>130</v>
+      </c>
+      <c r="B51" s="75" t="s">
+        <v>8</v>
+      </c>
+      <c r="C51" s="75" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" s="74" t="s">
-        <v>134</v>
-      </c>
-      <c r="B52" s="75" t="s">
-        <v>34</v>
-      </c>
-      <c r="C52" s="76"/>
+        <v>131</v>
+      </c>
+      <c r="B52" s="75">
+        <v>20</v>
+      </c>
+      <c r="C52" s="75">
+        <v>20</v>
+      </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" s="74" t="s">
-        <v>135</v>
-      </c>
-      <c r="B53" s="75">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="C53" s="76"/>
+        <v>132</v>
+      </c>
+      <c r="B53" s="75" t="s">
+        <v>34</v>
+      </c>
+      <c r="C53" s="75" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" s="74" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="B54" s="75">
-        <v>0</v>
-      </c>
-      <c r="C54" s="76"/>
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="C54" s="75">
+        <v>1.1000000000000001</v>
+      </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" s="74" t="s">
-        <v>137</v>
+        <v>218</v>
       </c>
       <c r="B55" s="75">
         <v>0</v>
       </c>
-      <c r="C55" s="76"/>
+      <c r="C55" s="75" t="s">
+        <v>220</v>
+      </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" s="74" t="s">
-        <v>138</v>
-      </c>
-      <c r="B56" s="75" t="s">
-        <v>8</v>
-      </c>
-      <c r="C56" s="76"/>
-    </row>
-    <row r="57" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B57" s="38"/>
-      <c r="C57" s="8"/>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A58" s="24" t="s">
-        <v>76</v>
-      </c>
-      <c r="B58" s="43"/>
-      <c r="C58" s="59"/>
+        <v>219</v>
+      </c>
+      <c r="B56" s="75">
+        <v>0</v>
+      </c>
+      <c r="C56" s="75" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57" s="74" t="s">
+        <v>134</v>
+      </c>
+      <c r="B57" s="75" t="s">
+        <v>8</v>
+      </c>
+      <c r="C57" s="75" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B58" s="38"/>
+      <c r="C58" s="8"/>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A59" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="B59" s="44" t="s">
-        <v>7</v>
-      </c>
-      <c r="C59" s="25"/>
+      <c r="A59" s="24" t="s">
+        <v>75</v>
+      </c>
+      <c r="B59" s="43"/>
+      <c r="C59" s="59"/>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="B60" s="44">
-        <v>2</v>
+        <v>55</v>
+      </c>
+      <c r="B60" s="44" t="s">
+        <v>7</v>
       </c>
       <c r="C60" s="25"/>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" s="6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B61" s="44">
-        <v>24</v>
+        <v>2</v>
       </c>
       <c r="C61" s="25"/>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="B62" s="44">
+        <v>24</v>
+      </c>
+      <c r="C62" s="25"/>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A63" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="B62" s="44">
+      <c r="B63" s="44">
         <v>20</v>
       </c>
-      <c r="C62" s="25"/>
-    </row>
-    <row r="63" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B63" s="38"/>
-      <c r="C63" s="8"/>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A64" s="20" t="s">
-        <v>77</v>
-      </c>
-      <c r="B64" s="45"/>
-      <c r="C64" s="60"/>
-    </row>
-    <row r="65" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="21" t="s">
-        <v>80</v>
-      </c>
-      <c r="B65" s="46">
-        <v>30</v>
-      </c>
-      <c r="C65" s="61"/>
+      <c r="C63" s="25"/>
+    </row>
+    <row r="64" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B64" s="38"/>
+      <c r="C64" s="8"/>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A65" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="B65" s="45"/>
+      <c r="C65" s="60"/>
     </row>
     <row r="66" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A66" s="21" t="s">
-        <v>81</v>
-      </c>
-      <c r="B66" s="46" t="s">
-        <v>7</v>
+        <v>79</v>
+      </c>
+      <c r="B66" s="46">
+        <v>30</v>
       </c>
       <c r="C66" s="61"/>
     </row>
     <row r="67" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A67" s="21" t="s">
-        <v>82</v>
-      </c>
-      <c r="B67" s="46">
-        <v>3.05</v>
+        <v>80</v>
+      </c>
+      <c r="B67" s="46" t="s">
+        <v>7</v>
       </c>
       <c r="C67" s="61"/>
     </row>
     <row r="68" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A68" s="21" t="s">
-        <v>114</v>
+        <v>81</v>
       </c>
       <c r="B68" s="46">
-        <v>20</v>
+        <v>3.05</v>
       </c>
       <c r="C68" s="61"/>
     </row>
     <row r="69" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A69" s="21" t="s">
-        <v>83</v>
+        <v>113</v>
       </c>
       <c r="B69" s="46">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="C69" s="61"/>
     </row>
     <row r="70" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A70" s="21" t="s">
-        <v>84</v>
-      </c>
-      <c r="B70" s="46" t="s">
-        <v>7</v>
+        <v>82</v>
+      </c>
+      <c r="B70" s="46">
+        <v>31</v>
       </c>
       <c r="C70" s="61"/>
     </row>
     <row r="71" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A71" s="21" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B71" s="46" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C71" s="61"/>
     </row>
     <row r="72" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A72" s="21" t="s">
-        <v>86</v>
-      </c>
-      <c r="B72" s="46">
-        <v>0.05</v>
+        <v>84</v>
+      </c>
+      <c r="B72" s="46" t="s">
+        <v>8</v>
       </c>
       <c r="C72" s="61"/>
     </row>
     <row r="73" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A73" s="21" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B73" s="46">
-        <v>3</v>
+        <v>0.05</v>
       </c>
       <c r="C73" s="61"/>
     </row>
     <row r="74" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A74" s="21" t="s">
-        <v>88</v>
-      </c>
-      <c r="B74" s="46" t="s">
-        <v>7</v>
+        <v>86</v>
+      </c>
+      <c r="B74" s="46">
+        <v>3</v>
       </c>
       <c r="C74" s="61"/>
     </row>
     <row r="75" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A75" s="21" t="s">
-        <v>89</v>
-      </c>
-      <c r="B75" s="46">
-        <v>1.4550000000000001</v>
+        <v>87</v>
+      </c>
+      <c r="B75" s="46" t="s">
+        <v>7</v>
       </c>
       <c r="C75" s="61"/>
     </row>
     <row r="76" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A76" s="21" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B76" s="46">
+        <v>1.4550000000000001</v>
+      </c>
+      <c r="C76" s="61"/>
+    </row>
+    <row r="77" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A77" s="21" t="s">
+        <v>89</v>
+      </c>
+      <c r="B77" s="46">
         <v>31</v>
-      </c>
-      <c r="C76" s="61"/>
-    </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A77" s="21" t="s">
-        <v>91</v>
-      </c>
-      <c r="B77" s="46" t="s">
-        <v>8</v>
       </c>
       <c r="C77" s="61"/>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" s="21" t="s">
-        <v>92</v>
-      </c>
-      <c r="B78" s="46">
-        <v>0.55500000000000005</v>
+        <v>90</v>
+      </c>
+      <c r="B78" s="46" t="s">
+        <v>8</v>
       </c>
       <c r="C78" s="61"/>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" s="21" t="s">
-        <v>124</v>
+        <v>91</v>
       </c>
       <c r="B79" s="46">
-        <v>0.5</v>
+        <v>0.55500000000000005</v>
       </c>
       <c r="C79" s="61"/>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" s="21" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="B80" s="46">
-        <v>1.75</v>
+        <v>0.5</v>
       </c>
       <c r="C80" s="61"/>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" s="21" t="s">
+        <v>123</v>
+      </c>
+      <c r="B81" s="46">
+        <v>1.75</v>
+      </c>
+      <c r="C81" s="61"/>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A82" s="21" t="s">
         <v>31</v>
       </c>
-      <c r="B81" s="46" t="s">
+      <c r="B82" s="46" t="s">
         <v>7</v>
       </c>
-      <c r="C81" s="61"/>
-    </row>
-    <row r="83" spans="1:3" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A83" s="26" t="s">
-        <v>79</v>
-      </c>
-      <c r="B83" s="48"/>
-      <c r="C83" s="27"/>
-    </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A84" s="28" t="s">
-        <v>39</v>
-      </c>
-      <c r="B84" s="49">
-        <v>0</v>
-      </c>
-      <c r="C84" s="29"/>
+      <c r="C82" s="61"/>
+    </row>
+    <row r="84" spans="1:3" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A84" s="26" t="s">
+        <v>78</v>
+      </c>
+      <c r="B84" s="48"/>
+      <c r="C84" s="27"/>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" s="28" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B85" s="49">
-        <v>-12</v>
+        <v>0</v>
       </c>
       <c r="C85" s="29"/>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86" s="28" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B86" s="49">
-        <v>-2</v>
+        <v>-12</v>
       </c>
       <c r="C86" s="29"/>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87" s="28" t="s">
-        <v>42</v>
-      </c>
-      <c r="B87" s="49" t="s">
-        <v>47</v>
+        <v>41</v>
+      </c>
+      <c r="B87" s="49">
+        <v>-2</v>
       </c>
       <c r="C87" s="29"/>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88" s="28" t="s">
-        <v>43</v>
-      </c>
-      <c r="B88" s="49">
-        <v>-0.2</v>
+        <v>42</v>
+      </c>
+      <c r="B88" s="49" t="s">
+        <v>47</v>
       </c>
       <c r="C88" s="29"/>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89" s="28" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B89" s="49">
-        <v>-1</v>
+        <v>-0.2</v>
       </c>
       <c r="C89" s="29"/>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90" s="28" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B90" s="49">
         <v>-1</v>
@@ -3097,68 +3266,77 @@
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91" s="28" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B91" s="49">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="C91" s="29"/>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92" s="28" t="s">
-        <v>123</v>
-      </c>
-      <c r="B92" s="49" t="s">
+        <v>46</v>
+      </c>
+      <c r="B92" s="49">
+        <v>0</v>
+      </c>
+      <c r="C92" s="29"/>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A93" s="28" t="s">
+        <v>121</v>
+      </c>
+      <c r="B93" s="49" t="s">
         <v>48</v>
       </c>
-      <c r="C92" s="29"/>
-    </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A94" s="34" t="s">
-        <v>78</v>
-      </c>
-      <c r="B94" s="50"/>
-      <c r="C94" s="30"/>
-    </row>
-    <row r="95" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A95" s="11" t="s">
+      <c r="C93" s="29"/>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A95" s="34" t="s">
+        <v>77</v>
+      </c>
+      <c r="B95" s="50"/>
+      <c r="C95" s="30"/>
+    </row>
+    <row r="96" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A96" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="B95" s="51" t="s">
-        <v>8</v>
-      </c>
-      <c r="C95" s="33"/>
-    </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A96" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="B96" s="51">
-        <v>5</v>
+      <c r="B96" s="51" t="s">
+        <v>8</v>
       </c>
       <c r="C96" s="33"/>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="B97" s="51" t="s">
-        <v>38</v>
+        <v>36</v>
+      </c>
+      <c r="B97" s="51">
+        <v>5</v>
       </c>
       <c r="C97" s="33"/>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98" s="11" t="s">
-        <v>116</v>
+        <v>37</v>
       </c>
       <c r="B98" s="51" t="s">
+        <v>38</v>
+      </c>
+      <c r="C98" s="33"/>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A99" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="B99" s="51" t="s">
         <v>33</v>
       </c>
-      <c r="C98" s="51"/>
+      <c r="C99" s="51"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B1">
-    <cfRule type="containsText" dxfId="10" priority="1" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="22" priority="1" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",B1)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
major update  - enabled multiprocessing for calc AAIMON ratios  - removed some folders, moved scripts to main directory  - renamed several files and functions  - added a list of acc where the SIMAP interface was successful, but the protein was not actually in their database
</commit_message>
<xml_diff>
--- a/korbinian/examples/settings/korbinian_run_settings_schweris.xlsx
+++ b/korbinian/examples/settings/korbinian_run_settings_schweris.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="17127"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="3090" yWindow="3135" windowWidth="14265" windowHeight="7680"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7995"/>
   </bookViews>
   <sheets>
     <sheet name="run_settings" sheetId="1" r:id="rId1"/>
@@ -687,7 +687,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1056,65 +1056,9 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="32">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="24">
     <dxf>
       <fill>
         <patternFill>
@@ -1303,9 +1247,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Larissa">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1343,9 +1287,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Larissa">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1378,9 +1322,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1413,9 +1374,26 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Larissa">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1591,11 +1569,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="59.42578125" style="1" customWidth="1"/>
     <col min="2" max="2" width="7.85546875" style="4" customWidth="1"/>
@@ -1626,7 +1604,7 @@
         <v>0</v>
       </c>
       <c r="B3" s="37">
-        <v>2</v>
+        <v>94</v>
       </c>
       <c r="C3" s="54" t="s">
         <v>9</v>
@@ -1773,7 +1751,7 @@
         <v>98</v>
       </c>
       <c r="B19" s="70" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C19" s="56" t="s">
         <v>15</v>
@@ -1784,7 +1762,7 @@
         <v>163</v>
       </c>
       <c r="B20" s="70" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C20" s="32" t="s">
         <v>16</v>
@@ -1817,7 +1795,7 @@
         <v>100</v>
       </c>
       <c r="B24" s="70" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C24" s="66" t="s">
         <v>18</v>
@@ -1839,7 +1817,7 @@
         <v>195</v>
       </c>
       <c r="B27" s="70" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C27" s="25" t="s">
         <v>196</v>
@@ -1861,7 +1839,7 @@
         <v>101</v>
       </c>
       <c r="B29" s="70" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C29" s="25" t="s">
         <v>62</v>
@@ -2013,103 +1991,103 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B1 B6 B45:B1048576">
-    <cfRule type="containsText" dxfId="31" priority="310" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="23" priority="301" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",B1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B21">
-    <cfRule type="containsText" dxfId="30" priority="308" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="22" priority="299" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",B21)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B25">
-    <cfRule type="containsText" dxfId="29" priority="307" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="21" priority="298" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",B25)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B32">
-    <cfRule type="containsText" dxfId="28" priority="306" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="20" priority="297" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",B32)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B37">
-    <cfRule type="containsText" dxfId="27" priority="305" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="19" priority="296" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",B37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B39:B44 B34 B36 B16:B17">
-    <cfRule type="containsText" dxfId="26" priority="304" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="18" priority="295" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",B16)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B35">
-    <cfRule type="containsText" dxfId="25" priority="294" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="17" priority="285" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",B35)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B31">
-    <cfRule type="containsText" dxfId="24" priority="237" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="16" priority="228" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",B31)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B18">
-    <cfRule type="containsText" dxfId="23" priority="228" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="15" priority="219" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",B18)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B13:B15">
-    <cfRule type="containsText" dxfId="22" priority="144" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="14" priority="135" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",B13)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B8:B10">
-    <cfRule type="containsText" dxfId="21" priority="113" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="13" priority="104" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",B8)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B11">
-    <cfRule type="containsText" dxfId="20" priority="112" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="12" priority="103" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",B11)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B23">
-    <cfRule type="containsText" dxfId="19" priority="76" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="11" priority="67" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",B23)))</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="B28">
+    <cfRule type="containsText" dxfId="10" priority="13" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",B28)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B19">
+    <cfRule type="containsText" dxfId="9" priority="11" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",B19)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B20">
+    <cfRule type="containsText" dxfId="8" priority="10" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",B20)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B24">
+    <cfRule type="containsText" dxfId="7" priority="9" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",B24)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B27">
+    <cfRule type="containsText" dxfId="6" priority="4" operator="containsText" text="TRUE">
+      <formula>NOT(ISERROR(SEARCH("TRUE",B27)))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="B30">
-    <cfRule type="containsText" dxfId="15" priority="11" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="5" priority="2" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",B30)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B29">
-    <cfRule type="containsText" dxfId="14" priority="7" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="4" priority="1" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",B29)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B28">
-    <cfRule type="containsText" dxfId="12" priority="5" operator="containsText" text="TRUE">
-      <formula>NOT(ISERROR(SEARCH("TRUE",B28)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B24">
-    <cfRule type="containsText" dxfId="7" priority="4" operator="containsText" text="TRUE">
-      <formula>NOT(ISERROR(SEARCH("TRUE",B24)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B27">
-    <cfRule type="containsText" dxfId="5" priority="3" operator="containsText" text="TRUE">
-      <formula>NOT(ISERROR(SEARCH("TRUE",B27)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B19">
-    <cfRule type="containsText" dxfId="3" priority="2" operator="containsText" text="TRUE">
-      <formula>NOT(ISERROR(SEARCH("TRUE",B19)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B20">
-    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="TRUE">
-      <formula>NOT(ISERROR(SEARCH("TRUE",B20)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2122,10 +2100,10 @@
   <dimension ref="A1:C23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="37.7109375" customWidth="1"/>
     <col min="2" max="2" width="71" customWidth="1"/>
@@ -2327,17 +2305,17 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B1">
-    <cfRule type="containsText" dxfId="11" priority="3" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="3" priority="3" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",B1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B15">
-    <cfRule type="containsText" dxfId="10" priority="2" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="2" priority="2" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",B15)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B16">
-    <cfRule type="containsText" dxfId="9" priority="1" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",B16)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2350,11 +2328,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C100"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="40.42578125" customWidth="1"/>
     <col min="2" max="2" width="31" style="47" customWidth="1"/>
@@ -3257,7 +3235,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B1">
-    <cfRule type="containsText" dxfId="8" priority="1" operator="containsText" text="TRUE">
+    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",B1)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>